<commit_message>
Update automatico via Actualizar 06-11-2020 17-09-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E55B322B-CF4D-4926-A633-631243DF318A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E28F61E5-2291-408E-AA8A-0F34572A5BDF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$522</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$527</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="E:\Comunicaciones REDD Dropbox\DI International\CORONAVIRUS\COVID_CL\Indicadores_Economicos_Chile_Reyes\IGPA.iqy" interval="60" name="IGPA" type="4" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" odcFile="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\IGPA.iqy" name="IGPA" type="4" refreshedVersion="6" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://si3.bcentral.cl/SieteIQY/secure/carga_series_excel.aspx" post="fechaInicio=[&quot;añoInicial&quot;,&quot;Año inicial&quot;]&amp;fechaFin=[&quot;añoFinal&quot;,&quot;Año final&quot;]&amp;param=WXB6UGl4OUojdDdqSkhoRSZ5T1BnNk9HVWwtJGImOTNSY0xTRSZQTnN4OWw3Ykh6VjUtc0ctVGx3ayY1ZEdHb3loJlN6MjJ4dTBSYnp4V0hEbiQycnFheXNZMzdMJGtCWmdPTkpSbEp3WVRaaiNoTDZkSmpxRFF6QTd6UW9xNCRZ" htmlTables="1" htmlFormat="all"/>
     <parameters count="2">
-      <parameter name="añoInicial" parameterType="value" string="2019"/>
-      <parameter name="añoFinal" parameterType="value" string="2020"/>
+      <parameter name="añoInicial" prompt="Año inicial"/>
+      <parameter name="añoFinal" prompt="Año final"/>
     </parameters>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,7 +621,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="IGPA" refreshOnLoad="1" preserveFormatting="0" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="IGPA" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,12 +920,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B522"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B527"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5107,7 +5105,48 @@
         <v>19502.54</v>
       </c>
     </row>
+    <row r="523" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A523" s="3">
+        <v>43987</v>
+      </c>
+      <c r="B523" s="4">
+        <v>20215.54</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A524" s="3">
+        <v>43988</v>
+      </c>
+      <c r="B524" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A525" s="3">
+        <v>43989</v>
+      </c>
+      <c r="B525" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A526" s="3">
+        <v>43990</v>
+      </c>
+      <c r="B526" s="4">
+        <v>20720.72</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A527" s="3">
+        <v>43991</v>
+      </c>
+      <c r="B527" s="4">
+        <v>20661.009999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 06-12-2020 17-05-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{669A9475-47BB-41BC-AC3E-C446667ED12D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$527</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$528</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\IGPA.iqy" name="IGPA" type="4" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\IGPA.iqy" name="IGPA" type="4" refreshedVersion="6" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://si3.bcentral.cl/SieteIQY/secure/carga_series_excel.aspx" post="fechaInicio=[&quot;añoInicial&quot;,&quot;Año inicial&quot;]&amp;fechaFin=[&quot;añoFinal&quot;,&quot;Año final&quot;]&amp;param=WXB6UGl4OUojdDdqSkhoRSZ5T1BnNk9HVWwtJGImOTNSY0xTRSZQTnN4OWw3Ykh6VjUtc0ctVGx3ayY1ZEdHb3loJlN6MjJ4dTBSYnp4V0hEbiQycnFheXNZMzdMJGtCWmdPTkpSbEp3WVRaaiNoTDZkSmpxRFF6QTd6UW9xNCRZ" htmlTables="1" htmlFormat="all"/>
     <parameters count="2">
       <parameter name="añoInicial" prompt="Año inicial"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,7 +621,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="IGPA" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="IGPA" preserveFormatting="0" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,10 +920,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B527"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B528"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
+      <selection activeCell="A530" sqref="A530"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5145,6 +5147,14 @@
         <v>20661.009999999998</v>
       </c>
     </row>
+    <row r="528" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A528" s="3">
+        <v>43992</v>
+      </c>
+      <c r="B528" s="4">
+        <v>20368.61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-13-2020 17-08-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{669A9475-47BB-41BC-AC3E-C446667ED12D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BB0BE51-90A9-4B0D-8A92-8F3FA12C396F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$528</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$529</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B528"/>
+  <dimension ref="A1:B529"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="A530" sqref="A530"/>
+      <selection activeCell="B532" sqref="B532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5155,6 +5155,14 @@
         <v>20368.61</v>
       </c>
     </row>
+    <row r="529" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A529" s="3">
+        <v>43993</v>
+      </c>
+      <c r="B529" s="4">
+        <v>19819.599999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-16-2020 00-40-24
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BB0BE51-90A9-4B0D-8A92-8F3FA12C396F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EBDEB47-637D-4FBA-A2C6-6334C683847B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$529</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$530</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,7 +921,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B529"/>
+  <dimension ref="A1:B530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
       <selection activeCell="B532" sqref="B532"/>
@@ -5163,6 +5163,14 @@
         <v>19819.599999999999</v>
       </c>
     </row>
+    <row r="530" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A530" s="3">
+        <v>43994</v>
+      </c>
+      <c r="B530" s="4">
+        <v>19990.189999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-17-2020 02-25-22
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EBDEB47-637D-4FBA-A2C6-6334C683847B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E0A9C19-8C7B-4DB7-8EFD-28FF202177DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="0" windowWidth="13296" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
@@ -924,7 +924,7 @@
   <dimension ref="A1:B530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="B532" sqref="B532"/>
+      <selection activeCell="B531" sqref="B531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-18-2020 02-16-41
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E0A9C19-8C7B-4DB7-8EFD-28FF202177DE}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{146B2D96-37DF-49C9-909C-0D9BF193430D}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="0" windowWidth="13296" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
@@ -924,7 +924,7 @@
   <dimension ref="A1:B530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="B531" sqref="B531"/>
+      <selection activeCell="B533" sqref="B533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-19-2020 02-20-45
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{146B2D96-37DF-49C9-909C-0D9BF193430D}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3195D9B8-AE3F-405C-A2E2-E32FC359A4D7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$530</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$535</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B530"/>
+  <dimension ref="A1:B535"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="B533" sqref="B533"/>
+      <selection activeCell="B537" sqref="B537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5171,6 +5171,46 @@
         <v>19990.189999999999</v>
       </c>
     </row>
+    <row r="531" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A531" s="3">
+        <v>43995</v>
+      </c>
+      <c r="B531" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A532" s="3">
+        <v>43996</v>
+      </c>
+      <c r="B532" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A533" s="3">
+        <v>43997</v>
+      </c>
+      <c r="B533" s="4">
+        <v>19587.27</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A534" s="3">
+        <v>43998</v>
+      </c>
+      <c r="B534" s="4">
+        <v>19806.400000000001</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A535" s="3">
+        <v>43999</v>
+      </c>
+      <c r="B535" s="4">
+        <v>20063.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-23-2020 17-08-27
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1ABBF50E-C639-4B61-9477-0F73F55ED9FB}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E00CC857-0E0B-4B45-8CE9-15FD91BF869A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="0" windowWidth="11496" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$535</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$537</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B535"/>
+  <dimension ref="A1:B537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="B537" sqref="B537"/>
+    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
+      <selection activeCell="A539" sqref="A539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5211,6 +5211,22 @@
         <v>20063.3</v>
       </c>
     </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A536" s="3">
+        <v>44000</v>
+      </c>
+      <c r="B536" s="4">
+        <v>20043.16</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A537" s="3">
+        <v>44001</v>
+      </c>
+      <c r="B537" s="4">
+        <v>20234.55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-24-2020 17-12-14
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E00CC857-0E0B-4B45-8CE9-15FD91BF869A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E95AFC0-851D-4768-9EB2-735BA8394062}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="0" windowWidth="11496" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-25-2020 17-09-35
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E95AFC0-851D-4768-9EB2-735BA8394062}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6774EF7B-F2F7-41FF-8ACE-38AFA4B3B8A2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$537</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$541</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B537"/>
+  <dimension ref="A1:B541"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A539" sqref="A539"/>
+      <selection activeCell="A543" sqref="A543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5227,6 +5227,38 @@
         <v>20234.55</v>
       </c>
     </row>
+    <row r="538" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A538" s="3">
+        <v>44002</v>
+      </c>
+      <c r="B538" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A539" s="3">
+        <v>44003</v>
+      </c>
+      <c r="B539" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A540" s="3">
+        <v>44004</v>
+      </c>
+      <c r="B540" s="4">
+        <v>20127.7</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A541" s="3">
+        <v>44005</v>
+      </c>
+      <c r="B541" s="4">
+        <v>20274.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2020 17-07-24
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6774EF7B-F2F7-41FF-8ACE-38AFA4B3B8A2}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13C7A464-F93C-4385-A934-E41BBAC37100}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$541</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$542</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B541"/>
+  <dimension ref="A1:B542"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A543" sqref="A543"/>
+      <selection activeCell="A544" sqref="A544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5259,6 +5259,14 @@
         <v>20274.84</v>
       </c>
     </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A542" s="3">
+        <v>44006</v>
+      </c>
+      <c r="B542" s="4">
+        <v>20295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-27-2020 17-09-38
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13C7A464-F93C-4385-A934-E41BBAC37100}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E8FAA3F-A80A-4E86-BF53-62E2D75C18DA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-01-2020 17-06-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E8FAA3F-A80A-4E86-BF53-62E2D75C18DA}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5D94F59-0AB1-4A51-95C6-07C68C66187F}"/>
   <bookViews>
-    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-02-2020 17-07-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5D94F59-0AB1-4A51-95C6-07C68C66187F}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E772EEE0-6959-42C5-856C-2C2B89A896A9}"/>
   <bookViews>
-    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7044" yWindow="0" windowWidth="15948" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-03-2020 17-06-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E772EEE0-6959-42C5-856C-2C2B89A896A9}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{413EA508-CEA3-43BE-A1C0-7A1905AC6BDC}"/>
   <bookViews>
-    <workbookView xWindow="7044" yWindow="0" windowWidth="15948" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$542</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$549</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B542"/>
+  <dimension ref="A1:B549"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A544" sqref="A544"/>
+      <selection activeCell="A551" sqref="A551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5267,6 +5267,62 @@
         <v>20295</v>
       </c>
     </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A543" s="3">
+        <v>44007</v>
+      </c>
+      <c r="B543" s="4">
+        <v>20306.740000000002</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A544" s="3">
+        <v>44008</v>
+      </c>
+      <c r="B544" s="4">
+        <v>20100.36</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A545" s="3">
+        <v>44009</v>
+      </c>
+      <c r="B545" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A546" s="3">
+        <v>44010</v>
+      </c>
+      <c r="B546" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A547" s="3">
+        <v>44011</v>
+      </c>
+      <c r="B547" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A548" s="3">
+        <v>44012</v>
+      </c>
+      <c r="B548" s="4">
+        <v>19969.02</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A549" s="3">
+        <v>44013</v>
+      </c>
+      <c r="B549" s="4">
+        <v>20315.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-04-2020 17-11-29
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{413EA508-CEA3-43BE-A1C0-7A1905AC6BDC}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{162F39D4-52DB-4FA2-B15B-3E9A75539D20}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$549</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$550</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B549"/>
+  <dimension ref="A1:B550"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A551" sqref="A551"/>
+      <selection activeCell="A553" sqref="A553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5323,6 +5323,14 @@
         <v>20315.63</v>
       </c>
     </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A550" s="3">
+        <v>44014</v>
+      </c>
+      <c r="B550" s="4">
+        <v>20996.17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-07-2020 17-07-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{162F39D4-52DB-4FA2-B15B-3E9A75539D20}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5AE7009-0FE7-4825-93A4-259B36E1783A}"/>
   <bookViews>
-    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9396" yWindow="0" windowWidth="13644" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$550</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$551</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B550"/>
+  <dimension ref="A1:B551"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A553" sqref="A553"/>
+      <selection activeCell="A554" sqref="A554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5331,6 +5331,14 @@
         <v>20996.17</v>
       </c>
     </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A551" s="3">
+        <v>44015</v>
+      </c>
+      <c r="B551" s="4">
+        <v>21147.759999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-08-2020 17-09-52
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5AE7009-0FE7-4825-93A4-259B36E1783A}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D87296B6-40D5-4D8D-BCCD-BFCA736736DE}"/>
   <bookViews>
-    <workbookView xWindow="9396" yWindow="0" windowWidth="13644" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$551</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$554</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B551"/>
+  <dimension ref="A1:B554"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A554" sqref="A554"/>
+      <selection activeCell="A556" sqref="A556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5339,6 +5339,30 @@
         <v>21147.759999999998</v>
       </c>
     </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A552" s="3">
+        <v>44016</v>
+      </c>
+      <c r="B552" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A553" s="3">
+        <v>44017</v>
+      </c>
+      <c r="B553" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A554" s="3">
+        <v>44018</v>
+      </c>
+      <c r="B554" s="4">
+        <v>21584.95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-09-2020 17-06-34
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D87296B6-40D5-4D8D-BCCD-BFCA736736DE}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5F82E731-30BF-423D-948F-36E3E09E80DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$554</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$555</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B554"/>
+  <dimension ref="A1:B555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A556" sqref="A556"/>
+    <sheetView tabSelected="1" topLeftCell="A540" workbookViewId="0">
+      <selection activeCell="A557" sqref="A557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5363,6 +5363,14 @@
         <v>21584.95</v>
       </c>
     </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A555" s="3">
+        <v>44019</v>
+      </c>
+      <c r="B555" s="4">
+        <v>21469.23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-17-2020 17-07-41
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC0CE27E-3B4F-45F8-B616-67CA0D7FB354}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{586E709F-F388-4BED-AF14-A34A5C580C23}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$683</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$684</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B683"/>
+  <dimension ref="A1:B684"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B670" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
+      <selection pane="bottomRight" activeCell="B684" sqref="B684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6398,6 +6398,14 @@
         <v>19601.240000000002</v>
       </c>
     </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="3">
+        <v>44148</v>
+      </c>
+      <c r="B684" s="4">
+        <v>19994.46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-02-2020 17-07-23
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D05D2E62-A30C-43A7-9BDF-4742CAF6AAC1}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF2CF1C2-9431-4D58-84F0-C4AF00E46985}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$698</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$701</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B698"/>
+  <dimension ref="A1:B701"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B688" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B698" sqref="B698"/>
+      <selection pane="bottomRight" activeCell="B701" sqref="B701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6518,6 +6518,30 @@
         <v>20593.349999999999</v>
       </c>
     </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="3">
+        <v>44163</v>
+      </c>
+      <c r="B699" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="3">
+        <v>44164</v>
+      </c>
+      <c r="B700" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="3">
+        <v>44165</v>
+      </c>
+      <c r="B701" s="4">
+        <v>20229.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-05-2020 17-07-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{996B8657-E379-4022-A797-809A6C17780B}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2D03191-BDBB-4910-ABF2-2476EC3B24FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$703</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$704</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B703"/>
+  <dimension ref="A1:B704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B694" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B703" sqref="B703"/>
+      <selection pane="bottomRight" activeCell="B704" sqref="B704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6558,6 +6558,14 @@
         <v>20769.53</v>
       </c>
     </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="3">
+        <v>44168</v>
+      </c>
+      <c r="B704" s="4">
+        <v>20929.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-08-2020 17-11-01
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2D03191-BDBB-4910-ABF2-2476EC3B24FE}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE68DD10-F151-4709-BC69-35C568F04406}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$704</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$705</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B704"/>
+  <dimension ref="A1:B705"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B694" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B700" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B704" sqref="B704"/>
+      <selection pane="bottomRight" activeCell="B705" sqref="B705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6566,6 +6566,14 @@
         <v>20929.88</v>
       </c>
     </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="3">
+        <v>44169</v>
+      </c>
+      <c r="B705" s="4">
+        <v>20933.36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-31-2020 17-11-38
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B42FA2C4-FB7F-4382-B59A-631522CDA9DD}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{50EC48BF-4CCE-4205-8014-518E34B2CEFE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$729</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$730</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B729"/>
+  <dimension ref="A1:B730"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B719" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B729" sqref="B729"/>
+      <selection pane="bottomRight" activeCell="B730" sqref="B730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6766,6 +6766,14 @@
         <v>20965.14</v>
       </c>
     </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="3">
+        <v>44194</v>
+      </c>
+      <c r="B730" s="4">
+        <v>21067.56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-31-2020 19-12-49
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{50EC48BF-4CCE-4205-8014-518E34B2CEFE}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{41269959-96FD-4903-8A5D-811965C88537}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A1:B730"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B719" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B725" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B730" sqref="B730"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-15-2021 20-54-08
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A7F55628-EC37-406E-980F-27E1BB9EDE5A}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{034AAF99-3EE9-4886-A53E-E1E8B4A6E4E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$745</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$746</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B745"/>
+  <dimension ref="A1:B746"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B745" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B745" sqref="B745"/>
+      <selection pane="bottomRight" activeCell="B746" sqref="B746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6894,6 +6894,14 @@
         <v>23314.21</v>
       </c>
     </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="3">
+        <v>44210</v>
+      </c>
+      <c r="B746" s="4">
+        <v>23260.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-21-2021 20-52-38
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IGPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64DF12C7-DE01-48AC-AE65-34A169ECD5A6}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{5431469F-1ACE-4607-9A59-3E6F814D6018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{102393DC-50B9-4583-853C-721DFFAEE7AD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IGPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$751</definedName>
+    <definedName name="IGPA" localSheetId="0">IGPA!$A$1:$B$752</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B751"/>
+  <dimension ref="A1:B752"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B745" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B751" sqref="B751"/>
+      <selection pane="bottomRight" activeCell="B752" sqref="B752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6942,6 +6942,14 @@
         <v>23438.85</v>
       </c>
     </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="3">
+        <v>44216</v>
+      </c>
+      <c r="B752" s="4">
+        <v>23329.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>